<commit_message>
too tired to write some commit, I hope we will ACE it tomorrow
</commit_message>
<xml_diff>
--- a/Documentation/Testing/CinemaSea_Testing_v.0.4.xlsx
+++ b/Documentation/Testing/CinemaSea_Testing_v.0.4.xlsx
@@ -2010,6 +2010,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="C23:E23"/>
@@ -2026,11 +2031,6 @@
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C15:E15"/>
     <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="C6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2053,8 +2053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D3:I96"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A78" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.25"/>
@@ -2983,7 +2983,7 @@
     </row>
     <row r="76" spans="4:9" ht="28.5" x14ac:dyDescent="0.25">
       <c r="D76" s="59">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E76" s="73" t="s">
         <v>215</v>

</xml_diff>